<commit_message>
Added Output Result File Code
</commit_message>
<xml_diff>
--- a/src/resources/Bandhan/DmiUrls.xlsx
+++ b/src/resources/Bandhan/DmiUrls.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratiksha.patil\Documents\Bandhan_Projects\Bandhan_DMI_URL_Automation\src\resources\Bandhan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing\Documents\Bandhan_DMI_URL_Automation\src\resources\Bandhan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB243D8-B2B5-4B7A-9D59-EF96BC1C1F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C15FE9B-5DC5-4D5E-8DEE-8F5E99601CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="55">
   <si>
     <t>SR_NO</t>
   </si>
@@ -113,6 +115,84 @@
   </si>
   <si>
     <t>https://marketplacetest.prowessbeat.net/bmart/Talwandi-Sabo/Rattangarh/411038/Wood-and-Timber-Contractor/DMI/c0fcd16a-db9b-48ba-973e-954f8009ef68</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?9071bd860983</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?84B815177218</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?d73ded6e4624</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?91a147623c4d</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?9b1f395ac9e6</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?983780248154</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?1b516e7c1af1</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?0f62027b52a2</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?72ce2b3cada5</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?7f6400c0f168</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?dd5c03bd74a0</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?8358f31b717a</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?41659712a405</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?bdfec7c0affc</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?f3d93a376bd7</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?879a21bc8982</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?862c0d103062</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?28a8fccbc657</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?1ee88c1a4aa9</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?98c7ad8e301b</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?c8825bad0bcc</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?67E6BEE85AFC</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?484AEE7D1231</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?bd3bffdd0128</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?e111eb28cf73</t>
+  </si>
+  <si>
+    <t>https://bandhan.prowessbeat.net/su?98ce1e6d67c2</t>
   </si>
 </sst>
 </file>
@@ -178,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -186,6 +266,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,20 +552,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="135.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="141.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,150 +576,1103 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>25</v>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
+      <c r="B9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4B6381-3A0E-4BED-B09E-B1CC7880E72E}">
+  <dimension ref="A1:C65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="141.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="7"/>
+    </row>
+  </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{314B6FD0-89C5-402E-A3F5-7939A0BE7F1D}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{2E904FB6-382A-4D7F-8A9C-9738E4F90FFC}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{3EDEED8B-6EA6-4548-9C7E-F1FDAC429C0F}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{314DECD2-6022-4946-8160-1CE267C270CE}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{0ED950A1-59A9-4890-8E25-AA3AB5E2DC4A}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{83C4C107-321C-4AF3-82E5-931DB461D76D}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{9E185C36-C3FA-45C3-8748-9652D77E9CBD}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{F151753A-9CF5-4D91-8404-125263179AE0}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{5C05E0E0-9ABB-41B8-BE1E-8D0C616C1084}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{7953D9FD-743E-4C20-B5B9-373FF21C24A0}"/>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{44CEB0D5-25DE-400B-8C53-3F48AEEC4C22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69C689B-4D3D-4560-8ECB-4FE47C9E2FBF}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="135.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DEDEA105-D237-4D16-AA72-86C2B1E11A75}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{AAED3B32-A793-4CE4-B221-B106944FE1F6}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{83E2582F-A49F-473B-9000-936F7C33D3BE}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{B4943628-A1E7-40DE-B03D-7C405F172C09}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{F4867A8C-DA9C-4251-9D77-CE22633C31D4}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{12952738-F7A8-4F64-8F95-58CE1279506F}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{A669D261-1E05-4FFF-B545-9FC09B78112A}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{39396FF4-523F-4F83-A5E5-1101014815F4}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{9FA28A4A-5419-4819-880A-5AC2B37B35A9}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{BF9CFB02-13B7-4A9E-834D-D37F32841038}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6678BC71-C337-4C51-BD16-2C11C492670C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
     <col min="2" max="2" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,7 +1683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -656,7 +1694,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -667,7 +1705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -678,7 +1716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -689,7 +1727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -700,7 +1738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -711,7 +1749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -722,7 +1760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -733,7 +1771,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -744,7 +1782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Update DMI URLs Input Excel File
</commit_message>
<xml_diff>
--- a/src/resources/Bandhan/DmiUrls.xlsx
+++ b/src/resources/Bandhan/DmiUrls.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing\Documents\Bandhan_DMI_URL_Automation\src\resources\Bandhan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C15FE9B-5DC5-4D5E-8DEE-8F5E99601CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5E041-F05D-4748-8757-4F4694659A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$C$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -199,16 +202,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,12 +219,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -256,21 +259,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -551,21 +553,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAF779-D041-4A9E-BEC5-A5458F2AECFA}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="141.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="141.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -576,408 +578,301 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" s="7"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" s="7"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B39" s="7"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" s="7"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" s="7"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" s="7"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" s="7"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="7"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="7"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="7"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="7"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="7"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="7"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="7"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="7"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="7"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="7"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="7"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="7"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="7"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{174CD21E-0D7D-46ED-97E1-39B3DC79565A}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{B049AF61-3553-4599-8558-59CD036488E8}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{FCCB2DAE-A2C4-4910-8390-04F8A2653F35}"/>
+    <hyperlink ref="B16" r:id="rId4" xr:uid="{9B149165-9A5E-472D-889A-7BCAC795362F}"/>
+    <hyperlink ref="B18" r:id="rId5" xr:uid="{AC52C012-EB19-4A2C-A8ED-DFEB5487B648}"/>
+    <hyperlink ref="B25" r:id="rId6" xr:uid="{0004DC15-9735-4464-99F7-4164F0AAB752}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -986,18 +881,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4B6381-3A0E-4BED-B09E-B1CC7880E72E}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="141.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="141.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1019,7 +914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1030,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1041,7 +936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1052,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1063,7 +958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1074,7 +969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1085,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1096,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1107,7 +1002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1118,7 +1013,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1127,7 +1022,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1136,7 +1031,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1145,7 +1040,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1154,7 +1049,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1163,7 +1058,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1172,7 +1067,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1181,7 +1076,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1190,7 +1085,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1199,7 +1094,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1208,7 +1103,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1217,7 +1112,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1226,7 +1121,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1235,7 +1130,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1244,7 +1139,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1253,7 +1148,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1262,7 +1157,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1271,7 +1166,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1280,16 +1175,16 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1298,7 +1193,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1307,7 +1202,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1316,7 +1211,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1325,7 +1220,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1334,7 +1229,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1343,7 +1238,7 @@
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1352,7 +1247,7 @@
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1361,7 +1256,7 @@
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1370,7 +1265,7 @@
       </c>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1379,7 +1274,7 @@
       </c>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1388,7 +1283,7 @@
       </c>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1397,7 +1292,7 @@
       </c>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1406,7 +1301,7 @@
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1415,7 +1310,7 @@
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1424,7 +1319,7 @@
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1433,7 +1328,7 @@
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1443,60 +1338,61 @@
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="7"/>
+      <c r="B48"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
+      <c r="B49"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
+      <c r="B50"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="7"/>
+      <c r="B51"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="7"/>
+      <c r="B52"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
+      <c r="B53"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="7"/>
+      <c r="B54"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="7"/>
+      <c r="B55"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="7"/>
+      <c r="B56"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="7"/>
+      <c r="B57"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="7"/>
+      <c r="B58"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="7"/>
+      <c r="B59"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="7"/>
+      <c r="B60"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="7"/>
+      <c r="B61"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="7"/>
+      <c r="B62"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="7"/>
+      <c r="B63"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="7"/>
+      <c r="B64"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="7"/>
+      <c r="B65"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C47" xr:uid="{5F4B6381-3A0E-4BED-B09E-B1CC7880E72E}"/>
   <hyperlinks>
     <hyperlink ref="B30" r:id="rId1" xr:uid="{44CEB0D5-25DE-400B-8C53-3F48AEEC4C22}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Added Selenium Grid Logic
</commit_message>
<xml_diff>
--- a/src/resources/Bandhan/DmiUrls.xlsx
+++ b/src/resources/Bandhan/DmiUrls.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5E041-F05D-4748-8757-4F4694659A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DE66A-0E41-43B2-88B2-3E370F32F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="DEV_URLS" sheetId="6" r:id="rId1"/>
+    <sheet name="PRODUCTION_URLS" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet5!$A$1:$C$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="125">
   <si>
     <t>SR_NO</t>
   </si>
@@ -196,6 +197,216 @@
   </si>
   <si>
     <t>https://bandhan.prowessbeat.net/su?98ce1e6d67c2</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?9be4fb046831</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?e06445c162c2</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?B9A8E9B7307C</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?1ea03f2241b0</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?f1a24aa26d55</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?212369eb0f7c</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?8f9e9db8a546</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?3f97f48bc0a6</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?c9bb06089b6d</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?fc32822f57e9</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?d6f164431e69</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?d2df2855b49a</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?50dfda9720da</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?028e64960e8e</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?fd2f75cf3ae1</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?15705b4435de</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?204dc1f31b11</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?d67f1d7681f6</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?6f7f7492ed33</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?77012f8df826</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?3d5783d82dc6</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?5447e02723bb</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?fb7751f3472b</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?4dc8e3b33495</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?f3ed19bfc06a</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b9b9d4de1964</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?5d46e3fd3d18</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?96c0bc1a1507</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?fccbb78684df</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b1b782e2e7d5</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?870e3130880c</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?030c2e75938c</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?c56319559b7e</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?59bc5bc84f99</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?9b73d56b23b5</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?00345db6dfae</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?2dfc84407a80</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?4fe76aa5793f</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?4ee7f1908d4c</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?f3a3fa4a1d7a</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b75b4d9337ff</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?4e7fc83b1bcd</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?8a8eb3d62b65</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?ec45782b9d4e</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?71905cbb1185</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?4160a5bfa9fd</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?70eac8799c13</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?6dc9c16fc98b</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b6e5e0c0d1b6</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?273116610d43</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b244a03b772f</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?67936046f9a7</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?f127ff2e0d03</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?24e6f9d7b8ef</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?0323f0e7c83c</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?16c8d8273515</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?78f00d5a2583</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?885f3fc7a8cf</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?b8f5a8c1f5e1</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?9c5a6cf1ce9e</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?9b4b0c1874a1</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?02c4b7adfdff</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?2a0d86975ea5</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?20dcff7c3b7e</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?47c287e2e3ff</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?d8e14e4511e7</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?3faec8b3ed6a</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?7b9a5c99ef17</t>
+  </si>
+  <si>
+    <t>https://bandhan.world/su/?1cdbe6c519b5</t>
+  </si>
+  <si>
+    <t>https://prowessbeat.net/?crXdRIIx</t>
   </si>
 </sst>
 </file>
@@ -556,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAF779-D041-4A9E-BEC5-A5458F2AECFA}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -878,6 +1089,809 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF3450E-966B-422C-83ED-F65DD981B2BA}">
+  <dimension ref="A1:C71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1DF7B4F0-5461-4020-9633-28B59110F7A4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4B6381-3A0E-4BED-B09E-B1CC7880E72E}">
   <dimension ref="A1:C65"/>
   <sheetViews>
@@ -1400,7 +2414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69C689B-4D3D-4560-8ECB-4FE47C9E2FBF}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1553,7 +2567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6678BC71-C337-4C51-BD16-2C11C492670C}">
   <dimension ref="A1:C11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update Code for Output Result Excel File
</commit_message>
<xml_diff>
--- a/src/resources/Bandhan/DmiUrls.xlsx
+++ b/src/resources/Bandhan/DmiUrls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DE66A-0E41-43B2-88B2-3E370F32F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A33D8DA-C6D9-4A33-9CAB-0B6D7AFE5BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV_URLS" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DEV_URLS!$A$1:$C$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PRODUCTION_URLS!$A$1:$C$71</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet5!$A$1:$C$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -413,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +431,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +465,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -484,6 +515,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -767,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAF779-D041-4A9E-BEC5-A5458F2AECFA}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,7 +839,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -815,7 +850,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -826,7 +861,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -848,7 +883,7 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -900,10 +935,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -914,7 +949,7 @@
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -933,10 +968,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -969,7 +1004,7 @@
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -991,7 +1026,7 @@
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1002,7 +1037,7 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1035,7 +1070,7 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1057,7 +1092,7 @@
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1076,6 +1111,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C27" xr:uid="{38CAF779-D041-4A9E-BEC5-A5458F2AECFA}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{174CD21E-0D7D-46ED-97E1-39B3DC79565A}"/>
     <hyperlink ref="B13" r:id="rId2" xr:uid="{B049AF61-3553-4599-8558-59CD036488E8}"/>
@@ -1092,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF3450E-966B-422C-83ED-F65DD981B2BA}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C71"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,7 +1164,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1139,7 +1175,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1150,7 +1186,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1161,7 +1197,7 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1799,7 +1835,7 @@
       <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="9" t="s">
         <v>117</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -1884,8 +1920,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C71" xr:uid="{8DF3450E-966B-422C-83ED-F65DD981B2BA}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{1DF7B4F0-5461-4020-9633-28B59110F7A4}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EE65F7AA-FE3D-4D5E-8F2E-318A4FADE89D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{14DFB585-E00D-4803-87C3-C72FEE0DED82}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{BD660930-BE8D-4D55-9691-12D7B1158089}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{D1C7006B-1059-41CF-B3E4-694D6380BEE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>